<commit_message>
edits to excel spreadsheets
</commit_message>
<xml_diff>
--- a/CurrentData/concerncombos.xlsx
+++ b/CurrentData/concerncombos.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="21">
   <si>
     <t>C1</t>
   </si>
@@ -80,6 +80,9 @@
   </si>
   <si>
     <t>TOTAL</t>
+  </si>
+  <si>
+    <t>Weighted by C1</t>
   </si>
 </sst>
 </file>
@@ -2323,15 +2326,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E71"/>
+  <dimension ref="A1:F71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G62" sqref="G62"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2347,1268 +2350,1554 @@
       <c r="E1" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="E2">
         <f>C2+D2</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="F2">
+        <f>E2/43</f>
+        <v>0.34883720930232559</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E66" si="0">C3+D3</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <f>C3+D3</f>
+        <v>33</v>
+      </c>
+      <c r="F3">
+        <f>E3/100</f>
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>56</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>194</v>
       </c>
       <c r="E4">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <f>C4+D4</f>
+        <v>250</v>
+      </c>
+      <c r="F4">
+        <f>E4/771</f>
+        <v>0.32425421530479898</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>147</v>
       </c>
       <c r="E5">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <f>C5+D5</f>
+        <v>187</v>
+      </c>
+      <c r="F5">
+        <f>E5/617</f>
+        <v>0.30307941653160453</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>7</v>
+      </c>
+      <c r="D6">
+        <v>13</v>
+      </c>
+      <c r="E6">
+        <f>C6+D6</f>
+        <v>20</v>
+      </c>
+      <c r="F6">
+        <f>E6/70</f>
+        <v>0.2857142857142857</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7">
+        <v>7</v>
+      </c>
+      <c r="D7">
+        <v>11</v>
+      </c>
+      <c r="E7">
+        <f>C7+D7</f>
+        <v>18</v>
+      </c>
+      <c r="F7">
+        <f>E7/65</f>
+        <v>0.27692307692307694</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8">
+        <v>23</v>
+      </c>
+      <c r="D8">
+        <v>44</v>
+      </c>
+      <c r="E8">
+        <f>C8+D8</f>
+        <v>67</v>
+      </c>
+      <c r="F8">
+        <f>E8/252</f>
+        <v>0.26587301587301587</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9">
+        <v>7</v>
+      </c>
+      <c r="D9">
+        <v>14</v>
+      </c>
+      <c r="E9">
+        <f>C9+D9</f>
+        <v>21</v>
+      </c>
+      <c r="F9">
+        <f>E9/81</f>
+        <v>0.25925925925925924</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10">
+        <v>13</v>
+      </c>
+      <c r="D10">
+        <v>52</v>
+      </c>
+      <c r="E10">
+        <f>C10+D10</f>
+        <v>65</v>
+      </c>
+      <c r="F10">
+        <f>E10/252</f>
+        <v>0.25793650793650796</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>8</v>
       </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6">
-        <v>2</v>
-      </c>
-      <c r="E6">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7">
-        <v>4</v>
-      </c>
-      <c r="D7">
-        <v>7</v>
-      </c>
-      <c r="E7">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11">
+        <v>5</v>
+      </c>
+      <c r="D11">
+        <v>13</v>
+      </c>
+      <c r="E11">
+        <f>C11+D11</f>
+        <v>18</v>
+      </c>
+      <c r="F11">
+        <f>E11/70</f>
+        <v>0.25714285714285712</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
+      <c r="D12">
+        <v>7</v>
+      </c>
+      <c r="E12">
+        <f>C12+D12</f>
+        <v>11</v>
+      </c>
+      <c r="F12">
+        <f>E12/43</f>
+        <v>0.2558139534883721</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
         <v>10</v>
       </c>
-      <c r="C8">
-        <v>2</v>
-      </c>
-      <c r="D8">
+      <c r="C13">
+        <v>29</v>
+      </c>
+      <c r="D13">
+        <v>80</v>
+      </c>
+      <c r="E13">
+        <f>C13+D13</f>
+        <v>109</v>
+      </c>
+      <c r="F13">
+        <f>E13/441</f>
+        <v>0.2471655328798186</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14">
+        <v>37</v>
+      </c>
+      <c r="D14">
+        <v>68</v>
+      </c>
+      <c r="E14">
+        <f>C14+D14</f>
+        <v>105</v>
+      </c>
+      <c r="F14">
+        <f>E14/441</f>
+        <v>0.23809523809523808</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15">
+        <v>10</v>
+      </c>
+      <c r="D15">
+        <v>30</v>
+      </c>
+      <c r="E15">
+        <f>C15+D15</f>
+        <v>40</v>
+      </c>
+      <c r="F15">
+        <f>E15/169</f>
+        <v>0.23668639053254437</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>13</v>
       </c>
-      <c r="E8">
-        <f t="shared" si="0"/>
+      <c r="B16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16">
+        <v>5</v>
+      </c>
+      <c r="D16">
+        <v>14</v>
+      </c>
+      <c r="E16">
+        <f>C16+D16</f>
+        <v>19</v>
+      </c>
+      <c r="F16">
+        <f>E16/81</f>
+        <v>0.23456790123456789</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17">
+        <v>49</v>
+      </c>
+      <c r="D17">
+        <v>95</v>
+      </c>
+      <c r="E17">
+        <f>C17+D17</f>
+        <v>144</v>
+      </c>
+      <c r="F17">
+        <f>E17/617</f>
+        <v>0.233387358184765</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18">
+        <v>18</v>
+      </c>
+      <c r="D18">
+        <v>19</v>
+      </c>
+      <c r="E18">
+        <f>C18+D18</f>
+        <v>37</v>
+      </c>
+      <c r="F18">
+        <f>E18/169</f>
+        <v>0.21893491124260356</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10">
-        <v>12</v>
-      </c>
-      <c r="D10">
-        <v>6</v>
-      </c>
-      <c r="E10">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11">
-        <v>26</v>
-      </c>
-      <c r="D11">
-        <v>59</v>
-      </c>
-      <c r="E11">
-        <f t="shared" si="0"/>
-        <v>85</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12">
-        <v>7</v>
-      </c>
-      <c r="E12">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13">
-        <v>13</v>
-      </c>
-      <c r="D13">
-        <v>17</v>
-      </c>
-      <c r="E13">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14">
-        <v>7</v>
-      </c>
-      <c r="D14">
-        <v>7</v>
-      </c>
-      <c r="E14">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15">
-        <v>26</v>
-      </c>
-      <c r="D15">
-        <v>14</v>
-      </c>
-      <c r="E15">
-        <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16">
-        <v>4</v>
-      </c>
-      <c r="D16">
-        <v>2</v>
-      </c>
-      <c r="E16">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17">
-        <v>19</v>
-      </c>
-      <c r="D17">
-        <v>23</v>
-      </c>
-      <c r="E17">
-        <f t="shared" si="0"/>
-        <v>42</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18">
-        <v>49</v>
-      </c>
-      <c r="D18">
-        <v>95</v>
-      </c>
-      <c r="E18">
-        <f t="shared" si="0"/>
-        <v>144</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>4</v>
       </c>
       <c r="B19" t="s">
         <v>10</v>
       </c>
       <c r="C19">
-        <v>40</v>
+        <v>2</v>
       </c>
       <c r="D19">
-        <v>147</v>
+        <v>32</v>
       </c>
       <c r="E19">
-        <f t="shared" si="0"/>
-        <v>187</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <f>C19+D19</f>
+        <v>34</v>
+      </c>
+      <c r="F19">
+        <f>E19/162</f>
+        <v>0.20987654320987653</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B20" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C20">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D20">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="E20">
-        <f t="shared" si="0"/>
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+        <f>C20+D20</f>
+        <v>18</v>
+      </c>
+      <c r="F20">
+        <f>E20/100</f>
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="B21" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C21">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D21">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E21">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+        <f>C21+D21</f>
+        <v>9</v>
+      </c>
+      <c r="F21">
+        <f>E21/65</f>
+        <v>0.13846153846153847</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B22" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C22">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="D22">
-        <v>3</v>
+        <v>59</v>
       </c>
       <c r="E22">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <f>C22+D22</f>
+        <v>85</v>
+      </c>
+      <c r="F22">
+        <f>E22/617</f>
+        <v>0.13776337115072934</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B23" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C23">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D23">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="E23">
-        <f t="shared" si="0"/>
+        <f>C23+D23</f>
+        <v>22</v>
+      </c>
+      <c r="F23">
+        <f>E23/162</f>
+        <v>0.13580246913580246</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24">
+        <v>7</v>
+      </c>
+      <c r="D24">
+        <v>12</v>
+      </c>
+      <c r="E24">
+        <f>C24+D24</f>
+        <v>19</v>
+      </c>
+      <c r="F24">
+        <f>E24/162</f>
+        <v>0.11728395061728394</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25">
+        <v>4</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <f>C25+D25</f>
+        <v>5</v>
+      </c>
+      <c r="F25">
+        <f>E25/43</f>
+        <v>0.11627906976744186</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="D26">
+        <v>7</v>
+      </c>
+      <c r="E26">
+        <f>C26+D26</f>
+        <v>9</v>
+      </c>
+      <c r="F26">
+        <f>E26/81</f>
+        <v>0.1111111111111111</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27">
+        <v>32</v>
+      </c>
+      <c r="D27">
+        <v>14</v>
+      </c>
+      <c r="E27">
+        <f>C27+D27</f>
+        <v>46</v>
+      </c>
+      <c r="F27">
+        <f>E27/441</f>
+        <v>0.10430839002267574</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>5</v>
-      </c>
-      <c r="B24" t="s">
+      <c r="B28" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
+      </c>
+      <c r="D28">
+        <v>5</v>
+      </c>
+      <c r="E28">
+        <f>C28+D28</f>
+        <v>7</v>
+      </c>
+      <c r="F28">
+        <f>E28/70</f>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29">
+        <v>22</v>
+      </c>
+      <c r="D29">
+        <v>49</v>
+      </c>
+      <c r="E29">
+        <f>C29+D29</f>
+        <v>71</v>
+      </c>
+      <c r="F29">
+        <f>E29/771</f>
+        <v>9.2088197146562911E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30">
+        <v>6</v>
+      </c>
+      <c r="D30">
+        <v>2</v>
+      </c>
+      <c r="E30">
+        <f>C30+D30</f>
         <v>8</v>
       </c>
-      <c r="C24">
-        <v>2</v>
-      </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
-      <c r="E24">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>5</v>
-      </c>
-      <c r="B25" t="s">
-        <v>15</v>
-      </c>
-      <c r="C25">
-        <v>2</v>
-      </c>
-      <c r="D25">
-        <v>1</v>
-      </c>
-      <c r="E25">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>5</v>
-      </c>
-      <c r="B26" t="s">
-        <v>9</v>
-      </c>
-      <c r="C26">
-        <v>7</v>
-      </c>
-      <c r="D26">
-        <v>11</v>
-      </c>
-      <c r="E26">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>5</v>
-      </c>
-      <c r="B27" t="s">
+      <c r="F30">
+        <f>E30/100</f>
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>12</v>
+      </c>
+      <c r="B31" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31">
+        <v>6</v>
+      </c>
+      <c r="D31">
+        <v>28</v>
+      </c>
+      <c r="E31">
+        <f>C31+D31</f>
+        <v>34</v>
+      </c>
+      <c r="F31">
+        <f>E31/441</f>
+        <v>7.7097505668934238E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>14</v>
+      </c>
+      <c r="B32" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32">
+        <v>2</v>
+      </c>
+      <c r="D32">
+        <v>3</v>
+      </c>
+      <c r="E32">
+        <f>C32+D32</f>
+        <v>5</v>
+      </c>
+      <c r="F32">
+        <f>E32/65</f>
+        <v>7.6923076923076927E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>10</v>
       </c>
-      <c r="C27">
-        <v>12</v>
-      </c>
-      <c r="D27">
-        <v>21</v>
-      </c>
-      <c r="E27">
-        <f t="shared" si="0"/>
-        <v>33</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>12</v>
-      </c>
-      <c r="B28" t="s">
-        <v>5</v>
-      </c>
-      <c r="C28">
-        <v>4</v>
-      </c>
-      <c r="D28">
-        <v>1</v>
-      </c>
-      <c r="E28">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>12</v>
-      </c>
-      <c r="B29" t="s">
+      <c r="B33" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33">
+        <v>50</v>
+      </c>
+      <c r="D33">
+        <v>14</v>
+      </c>
+      <c r="E33">
+        <f>C33+D33</f>
+        <v>64</v>
+      </c>
+      <c r="F33">
+        <f>E33/856</f>
+        <v>7.476635514018691E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>13</v>
-      </c>
-      <c r="C29">
-        <v>2</v>
-      </c>
-      <c r="D29">
-        <v>6</v>
-      </c>
-      <c r="E29">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>12</v>
-      </c>
-      <c r="B30" t="s">
-        <v>6</v>
-      </c>
-      <c r="C30">
-        <v>32</v>
-      </c>
-      <c r="D30">
-        <v>14</v>
-      </c>
-      <c r="E30">
-        <f t="shared" si="0"/>
-        <v>46</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>12</v>
-      </c>
-      <c r="B31" t="s">
-        <v>14</v>
-      </c>
-      <c r="C31">
-        <v>9</v>
-      </c>
-      <c r="D31">
-        <v>2</v>
-      </c>
-      <c r="E31">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>12</v>
-      </c>
-      <c r="B32" t="s">
-        <v>7</v>
-      </c>
-      <c r="C32">
-        <v>9</v>
-      </c>
-      <c r="D32">
-        <v>5</v>
-      </c>
-      <c r="E32">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>12</v>
-      </c>
-      <c r="B33" t="s">
-        <v>8</v>
-      </c>
-      <c r="C33">
-        <v>5</v>
-      </c>
-      <c r="D33">
-        <v>1</v>
-      </c>
-      <c r="E33">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>12</v>
       </c>
       <c r="B34" t="s">
         <v>15</v>
       </c>
       <c r="C34">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D34">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E34">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+        <f>C34+D34</f>
+        <v>6</v>
+      </c>
+      <c r="F34">
+        <f>E34/81</f>
+        <v>7.407407407407407E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B35" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C35">
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="D35">
-        <v>68</v>
+        <v>3</v>
       </c>
       <c r="E35">
-        <f t="shared" si="0"/>
-        <v>105</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+        <f>C35+D35</f>
+        <v>7</v>
+      </c>
+      <c r="F35">
+        <f>E35/100</f>
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="B36" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C36">
-        <v>29</v>
+        <v>2</v>
       </c>
       <c r="D36">
-        <v>80</v>
+        <v>1</v>
       </c>
       <c r="E36">
-        <f t="shared" si="0"/>
-        <v>109</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+        <f>C36+D36</f>
+        <v>3</v>
+      </c>
+      <c r="F36">
+        <f>E36/43</f>
+        <v>6.9767441860465115E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="B37" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C37">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D37">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="E37">
-        <f t="shared" si="0"/>
-        <v>34</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+        <f>C37+D37</f>
+        <v>3</v>
+      </c>
+      <c r="F37">
+        <f>E37/43</f>
+        <v>6.9767441860465115E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="B38" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C38">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="D38">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="E38">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+        <f>C38+D38</f>
+        <v>42</v>
+      </c>
+      <c r="F38">
+        <f>E38/617</f>
+        <v>6.8071312803889783E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="B39" t="s">
         <v>7</v>
       </c>
       <c r="C39">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="D39">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="E39">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+        <f>C39+D39</f>
+        <v>40</v>
+      </c>
+      <c r="F39">
+        <f>E39/617</f>
+        <v>6.4829821717990274E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>13</v>
       </c>
       <c r="B40" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C40">
         <v>4</v>
       </c>
       <c r="D40">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E40">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+        <f>C40+D40</f>
+        <v>5</v>
+      </c>
+      <c r="F40">
+        <f>E40/81</f>
+        <v>6.1728395061728392E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="B41" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C41">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D41">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="E41">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+        <f>C41+D41</f>
+        <v>38</v>
+      </c>
+      <c r="F41">
+        <f>E41/617</f>
+        <v>6.1588330632090758E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B42" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C42">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D42">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="E42">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+        <f>C42+D42</f>
+        <v>6</v>
+      </c>
+      <c r="F42">
+        <f>E42/100</f>
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>13</v>
       </c>
       <c r="B43" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C43">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D43">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E43">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+        <f>C43+D43</f>
+        <v>4</v>
+      </c>
+      <c r="F43">
+        <f>E43/81</f>
+        <v>4.9382716049382713E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B44" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C44">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D44">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="E44">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+        <f>C44+D44</f>
+        <v>30</v>
+      </c>
+      <c r="F44">
+        <f>E44/617</f>
+        <v>4.8622366288492709E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B45" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C45">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D45">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E45">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+        <f>C45+D45</f>
+        <v>8</v>
+      </c>
+      <c r="F45">
+        <f>E45/169</f>
+        <v>4.7337278106508875E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B46" t="s">
+        <v>5</v>
+      </c>
+      <c r="C46">
+        <v>2</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+      <c r="E46">
+        <f>C46+D46</f>
+        <v>2</v>
+      </c>
+      <c r="F46">
+        <f>E46/43</f>
+        <v>4.6511627906976744E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>3</v>
+      </c>
+      <c r="B47" t="s">
+        <v>7</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="E47">
+        <f>C47+D47</f>
+        <v>2</v>
+      </c>
+      <c r="F47">
+        <f>E47/43</f>
+        <v>4.6511627906976744E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>14</v>
+      </c>
+      <c r="B48" t="s">
         <v>8</v>
       </c>
-      <c r="C46">
-        <v>1</v>
-      </c>
-      <c r="D46">
-        <v>2</v>
-      </c>
-      <c r="E46">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>6</v>
-      </c>
-      <c r="B47" t="s">
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="D48">
+        <v>2</v>
+      </c>
+      <c r="E48">
+        <f>C48+D48</f>
+        <v>3</v>
+      </c>
+      <c r="F48">
+        <f>E48/65</f>
+        <v>4.6153846153846156E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>14</v>
+      </c>
+      <c r="B49" t="s">
         <v>15</v>
       </c>
-      <c r="C47">
-        <v>6</v>
-      </c>
-      <c r="D47">
-        <v>2</v>
-      </c>
-      <c r="E47">
-        <f t="shared" si="0"/>
+      <c r="C49">
+        <v>2</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
+      <c r="E49">
+        <f>C49+D49</f>
+        <v>3</v>
+      </c>
+      <c r="F49">
+        <f>E49/65</f>
+        <v>4.6153846153846156E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>7</v>
+      </c>
+      <c r="B50" t="s">
+        <v>15</v>
+      </c>
+      <c r="C50">
+        <v>2</v>
+      </c>
+      <c r="D50">
+        <v>5</v>
+      </c>
+      <c r="E50">
+        <f>C50+D50</f>
+        <v>7</v>
+      </c>
+      <c r="F50">
+        <f>E50/169</f>
+        <v>4.142011834319527E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>12</v>
+      </c>
+      <c r="B51" t="s">
+        <v>15</v>
+      </c>
+      <c r="C51">
+        <v>12</v>
+      </c>
+      <c r="D51">
+        <v>5</v>
+      </c>
+      <c r="E51">
+        <f>C51+D51</f>
+        <v>17</v>
+      </c>
+      <c r="F51">
+        <f>E51/441</f>
+        <v>3.8548752834467119E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>6</v>
+      </c>
+      <c r="B52" t="s">
+        <v>11</v>
+      </c>
+      <c r="C52">
+        <v>3</v>
+      </c>
+      <c r="D52">
+        <v>6</v>
+      </c>
+      <c r="E52">
+        <f>C52+D52</f>
+        <v>9</v>
+      </c>
+      <c r="F52">
+        <f>E52/252</f>
+        <v>3.5714285714285712E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>12</v>
+      </c>
+      <c r="B53" t="s">
+        <v>7</v>
+      </c>
+      <c r="C53">
+        <v>9</v>
+      </c>
+      <c r="D53">
+        <v>5</v>
+      </c>
+      <c r="E53">
+        <f>C53+D53</f>
+        <v>14</v>
+      </c>
+      <c r="F53">
+        <f>E53/441</f>
+        <v>3.1746031746031744E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>6</v>
+      </c>
+      <c r="B54" t="s">
+        <v>15</v>
+      </c>
+      <c r="C54">
+        <v>6</v>
+      </c>
+      <c r="D54">
+        <v>2</v>
+      </c>
+      <c r="E54">
+        <f>C54+D54</f>
         <v>8</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>6</v>
-      </c>
-      <c r="B48" t="s">
-        <v>9</v>
-      </c>
-      <c r="C48">
-        <v>23</v>
-      </c>
-      <c r="D48">
-        <v>44</v>
-      </c>
-      <c r="E48">
-        <f t="shared" si="0"/>
-        <v>67</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>6</v>
-      </c>
-      <c r="B49" t="s">
-        <v>10</v>
-      </c>
-      <c r="C49">
+      <c r="F54">
+        <f>E54/252</f>
+        <v>3.1746031746031744E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>5</v>
+      </c>
+      <c r="B55" t="s">
+        <v>15</v>
+      </c>
+      <c r="C55">
+        <v>2</v>
+      </c>
+      <c r="D55">
+        <v>1</v>
+      </c>
+      <c r="E55">
+        <f>C55+D55</f>
+        <v>3</v>
+      </c>
+      <c r="F55">
+        <f>E55/100</f>
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>4</v>
+      </c>
+      <c r="B56" t="s">
+        <v>5</v>
+      </c>
+      <c r="C56">
+        <v>12</v>
+      </c>
+      <c r="D56">
+        <v>6</v>
+      </c>
+      <c r="E56">
+        <f>C56+D56</f>
+        <v>18</v>
+      </c>
+      <c r="F56">
+        <f>E56/617</f>
+        <v>2.9173419773095625E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>6</v>
+      </c>
+      <c r="B57" t="s">
+        <v>7</v>
+      </c>
+      <c r="C57">
+        <v>3</v>
+      </c>
+      <c r="D57">
+        <v>4</v>
+      </c>
+      <c r="E57">
+        <f>C57+D57</f>
+        <v>7</v>
+      </c>
+      <c r="F57">
+        <f>E57/252</f>
+        <v>2.7777777777777776E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>12</v>
+      </c>
+      <c r="B58" t="s">
+        <v>14</v>
+      </c>
+      <c r="C58">
+        <v>9</v>
+      </c>
+      <c r="D58">
+        <v>2</v>
+      </c>
+      <c r="E58">
+        <f>C58+D58</f>
+        <v>11</v>
+      </c>
+      <c r="F58">
+        <f>E58/441</f>
+        <v>2.4943310657596373E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>3</v>
+      </c>
+      <c r="B59" t="s">
+        <v>11</v>
+      </c>
+      <c r="C59">
+        <v>1</v>
+      </c>
+      <c r="D59">
+        <v>0</v>
+      </c>
+      <c r="E59">
+        <f>C59+D59</f>
+        <v>1</v>
+      </c>
+      <c r="F59">
+        <f>E59/43</f>
+        <v>2.3255813953488372E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>4</v>
+      </c>
+      <c r="B60" t="s">
+        <v>14</v>
+      </c>
+      <c r="C60">
+        <v>7</v>
+      </c>
+      <c r="D60">
+        <v>7</v>
+      </c>
+      <c r="E60">
+        <f>C60+D60</f>
+        <v>14</v>
+      </c>
+      <c r="F60">
+        <f>E60/617</f>
+        <v>2.2690437601296597E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>5</v>
+      </c>
+      <c r="B61" t="s">
+        <v>8</v>
+      </c>
+      <c r="C61">
+        <v>2</v>
+      </c>
+      <c r="D61">
+        <v>0</v>
+      </c>
+      <c r="E61">
+        <f>C61+D61</f>
+        <v>2</v>
+      </c>
+      <c r="F61">
+        <f>E61/100</f>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>12</v>
+      </c>
+      <c r="B62" t="s">
         <v>13</v>
       </c>
-      <c r="D49">
-        <v>52</v>
-      </c>
-      <c r="E49">
-        <f t="shared" si="0"/>
-        <v>65</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>6</v>
-      </c>
-      <c r="B50" t="s">
-        <v>11</v>
-      </c>
-      <c r="C50">
-        <v>3</v>
-      </c>
-      <c r="D50">
-        <v>6</v>
-      </c>
-      <c r="E50">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>14</v>
-      </c>
-      <c r="B51" t="s">
+      <c r="C62">
+        <v>2</v>
+      </c>
+      <c r="D62">
+        <v>6</v>
+      </c>
+      <c r="E62">
+        <f>C62+D62</f>
         <v>8</v>
       </c>
-      <c r="C51">
-        <v>1</v>
-      </c>
-      <c r="D51">
-        <v>2</v>
-      </c>
-      <c r="E51">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>14</v>
-      </c>
-      <c r="B52" t="s">
+      <c r="F62">
+        <f>E62/441</f>
+        <v>1.8140589569160998E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>12</v>
+      </c>
+      <c r="B63" t="s">
+        <v>8</v>
+      </c>
+      <c r="C63">
+        <v>5</v>
+      </c>
+      <c r="D63">
+        <v>1</v>
+      </c>
+      <c r="E63">
+        <f>C63+D63</f>
+        <v>6</v>
+      </c>
+      <c r="F63">
+        <f>E63/441</f>
+        <v>1.3605442176870748E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>4</v>
+      </c>
+      <c r="B64" t="s">
+        <v>13</v>
+      </c>
+      <c r="C64">
+        <v>1</v>
+      </c>
+      <c r="D64">
+        <v>7</v>
+      </c>
+      <c r="E64">
+        <f>C64+D64</f>
+        <v>8</v>
+      </c>
+      <c r="F64">
+        <f>E64/617</f>
+        <v>1.2965964343598054E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>6</v>
+      </c>
+      <c r="B65" t="s">
+        <v>8</v>
+      </c>
+      <c r="C65">
+        <v>1</v>
+      </c>
+      <c r="D65">
+        <v>2</v>
+      </c>
+      <c r="E65">
+        <f>C65+D65</f>
+        <v>3</v>
+      </c>
+      <c r="F65">
+        <f>E65/252</f>
+        <v>1.1904761904761904E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>7</v>
+      </c>
+      <c r="B66" t="s">
+        <v>8</v>
+      </c>
+      <c r="C66">
+        <v>2</v>
+      </c>
+      <c r="D66">
+        <v>0</v>
+      </c>
+      <c r="E66">
+        <f>C66+D66</f>
+        <v>2</v>
+      </c>
+      <c r="F66">
+        <f>E66/169</f>
+        <v>1.1834319526627219E-2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>12</v>
+      </c>
+      <c r="B67" t="s">
+        <v>5</v>
+      </c>
+      <c r="C67">
+        <v>4</v>
+      </c>
+      <c r="D67">
+        <v>1</v>
+      </c>
+      <c r="E67">
+        <f>C67+D67</f>
+        <v>5</v>
+      </c>
+      <c r="F67">
+        <f>E67/441</f>
+        <v>1.1337868480725623E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>4</v>
+      </c>
+      <c r="B68" t="s">
+        <v>8</v>
+      </c>
+      <c r="C68">
+        <v>4</v>
+      </c>
+      <c r="D68">
+        <v>2</v>
+      </c>
+      <c r="E68">
+        <f>C68+D68</f>
+        <v>6</v>
+      </c>
+      <c r="F68">
+        <f>E68/617</f>
+        <v>9.7244732576985422E-3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>6</v>
+      </c>
+      <c r="B69" t="s">
+        <v>14</v>
+      </c>
+      <c r="C69">
+        <v>1</v>
+      </c>
+      <c r="D69">
+        <v>1</v>
+      </c>
+      <c r="E69">
+        <f>C69+D69</f>
+        <v>2</v>
+      </c>
+      <c r="F69">
+        <f>E69/252</f>
+        <v>7.9365079365079361E-3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>11</v>
+      </c>
+      <c r="B70" t="s">
+        <v>5</v>
+      </c>
+      <c r="C70">
+        <v>2</v>
+      </c>
+      <c r="D70">
+        <v>0</v>
+      </c>
+      <c r="E70">
+        <f>C70+D70</f>
+        <v>2</v>
+      </c>
+      <c r="F70">
+        <f>E70/267</f>
+        <v>7.4906367041198503E-3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
         <v>15</v>
       </c>
-      <c r="C52">
-        <v>2</v>
-      </c>
-      <c r="D52">
-        <v>1</v>
-      </c>
-      <c r="E52">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>14</v>
-      </c>
-      <c r="B53" t="s">
-        <v>9</v>
-      </c>
-      <c r="C53">
-        <v>4</v>
-      </c>
-      <c r="D53">
-        <v>5</v>
-      </c>
-      <c r="E53">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>14</v>
-      </c>
-      <c r="B54" t="s">
-        <v>10</v>
-      </c>
-      <c r="C54">
-        <v>7</v>
-      </c>
-      <c r="D54">
-        <v>11</v>
-      </c>
-      <c r="E54">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>14</v>
-      </c>
-      <c r="B55" t="s">
-        <v>11</v>
-      </c>
-      <c r="C55">
-        <v>2</v>
-      </c>
-      <c r="D55">
-        <v>3</v>
-      </c>
-      <c r="E55">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>7</v>
-      </c>
-      <c r="B56" t="s">
-        <v>8</v>
-      </c>
-      <c r="C56">
-        <v>2</v>
-      </c>
-      <c r="D56">
-        <v>0</v>
-      </c>
-      <c r="E56">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>7</v>
-      </c>
-      <c r="B57" t="s">
-        <v>15</v>
-      </c>
-      <c r="C57">
-        <v>2</v>
-      </c>
-      <c r="D57">
-        <v>5</v>
-      </c>
-      <c r="E57">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>7</v>
-      </c>
-      <c r="B58" t="s">
-        <v>9</v>
-      </c>
-      <c r="C58">
-        <v>18</v>
-      </c>
-      <c r="D58">
-        <v>19</v>
-      </c>
-      <c r="E58">
-        <f t="shared" si="0"/>
-        <v>37</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>7</v>
-      </c>
-      <c r="B59" t="s">
-        <v>10</v>
-      </c>
-      <c r="C59">
-        <v>10</v>
-      </c>
-      <c r="D59">
-        <v>30</v>
-      </c>
-      <c r="E59">
-        <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>7</v>
-      </c>
-      <c r="B60" t="s">
-        <v>11</v>
-      </c>
-      <c r="C60">
-        <v>2</v>
-      </c>
-      <c r="D60">
-        <v>6</v>
-      </c>
-      <c r="E60">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>8</v>
-      </c>
-      <c r="B61" t="s">
-        <v>9</v>
-      </c>
-      <c r="C61">
-        <v>5</v>
-      </c>
-      <c r="D61">
-        <v>13</v>
-      </c>
-      <c r="E61">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>8</v>
-      </c>
-      <c r="B62" t="s">
-        <v>10</v>
-      </c>
-      <c r="C62">
-        <v>7</v>
-      </c>
-      <c r="D62">
-        <v>13</v>
-      </c>
-      <c r="E62">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>8</v>
-      </c>
-      <c r="B63" t="s">
-        <v>11</v>
-      </c>
-      <c r="C63">
-        <v>2</v>
-      </c>
-      <c r="D63">
-        <v>5</v>
-      </c>
-      <c r="E63">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>15</v>
-      </c>
-      <c r="B64" t="s">
-        <v>3</v>
-      </c>
-      <c r="C64">
-        <v>1</v>
-      </c>
-      <c r="D64">
-        <v>0</v>
-      </c>
-      <c r="E64">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>15</v>
-      </c>
-      <c r="B65" t="s">
-        <v>9</v>
-      </c>
-      <c r="C65">
-        <v>10</v>
-      </c>
-      <c r="D65">
-        <v>12</v>
-      </c>
-      <c r="E65">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>15</v>
-      </c>
-      <c r="B66" t="s">
-        <v>10</v>
-      </c>
-      <c r="C66">
-        <v>2</v>
-      </c>
-      <c r="D66">
-        <v>32</v>
-      </c>
-      <c r="E66">
-        <f t="shared" si="0"/>
-        <v>34</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>15</v>
-      </c>
-      <c r="B67" t="s">
-        <v>11</v>
-      </c>
-      <c r="C67">
-        <v>7</v>
-      </c>
-      <c r="D67">
-        <v>12</v>
-      </c>
-      <c r="E67">
-        <f t="shared" ref="E67:E71" si="1">C67+D67</f>
-        <v>19</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>9</v>
-      </c>
-      <c r="B68" t="s">
-        <v>10</v>
-      </c>
-      <c r="C68">
-        <v>56</v>
-      </c>
-      <c r="D68">
-        <v>194</v>
-      </c>
-      <c r="E68">
-        <f t="shared" si="1"/>
-        <v>250</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>9</v>
-      </c>
-      <c r="B69" t="s">
-        <v>11</v>
-      </c>
-      <c r="C69">
-        <v>22</v>
-      </c>
-      <c r="D69">
-        <v>49</v>
-      </c>
-      <c r="E69">
-        <f t="shared" si="1"/>
-        <v>71</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>10</v>
-      </c>
-      <c r="B70" t="s">
-        <v>11</v>
-      </c>
-      <c r="C70">
-        <v>50</v>
-      </c>
-      <c r="D70">
-        <v>14</v>
-      </c>
-      <c r="E70">
-        <f t="shared" si="1"/>
-        <v>64</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>11</v>
-      </c>
       <c r="B71" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C71">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D71">
         <v>0</v>
       </c>
       <c r="E71">
-        <f t="shared" si="1"/>
-        <v>2</v>
+        <f>C71+D71</f>
+        <v>1</v>
+      </c>
+      <c r="F71">
+        <f>E71/162</f>
+        <v>6.1728395061728392E-3</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:F71">
+    <sortCondition descending="1" ref="F2:F71"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>